<commit_message>
Upload first pass at parser.
</commit_message>
<xml_diff>
--- a/pyfair/static/data_entry.xlsx
+++ b/pyfair/static/data_entry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theon\development\pyfair\pyfair\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3646B-E53E-4B60-9FC3-E3E408AA42DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D757FCE-AC0C-4288-9144-E679854C5BC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11050" yWindow="4720" windowWidth="19030" windowHeight="14070" activeTab="1" xr2:uid="{76265505-8B04-4CE4-A2A8-932A5C405433}"/>
+    <workbookView xWindow="0" yWindow="370" windowWidth="19030" windowHeight="14070" xr2:uid="{76265505-8B04-4CE4-A2A8-932A5C405433}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="33">
   <si>
     <t>Loss Event Frequency</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Model Name</t>
-  </si>
-  <si>
-    <t>Author</t>
   </si>
   <si>
     <t>Number of Simulations</t>
@@ -660,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA18B4-909D-485F-BD49-3CA8F97B191F}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,63 +672,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="14">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="18" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="C7" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
       <c r="C8" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="C9" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="C9" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
       <c r="C10" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="C11" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78B95C9-ABB7-49B9-AE9D-BEB6D66B5BF4}">
   <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -758,10 +751,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>20</v>
@@ -776,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>12</v>
@@ -966,10 +959,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>20</v>
@@ -984,7 +977,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>12</v>
@@ -1174,10 +1167,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>20</v>
@@ -1192,7 +1185,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>12</v>
@@ -1382,10 +1375,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>20</v>
@@ -1400,7 +1393,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>12</v>
@@ -1590,10 +1583,10 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>20</v>
@@ -1608,7 +1601,7 @@
         <v>11</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>12</v>
@@ -1798,10 +1791,10 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>20</v>
@@ -1816,7 +1809,7 @@
         <v>11</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>12</v>
@@ -2006,10 +1999,10 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>20</v>
@@ -2024,7 +2017,7 @@
         <v>11</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>12</v>
@@ -2214,10 +2207,10 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>20</v>
@@ -2232,7 +2225,7 @@
         <v>11</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I85" s="7" t="s">
         <v>12</v>
@@ -2422,10 +2415,10 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>20</v>
@@ -2440,7 +2433,7 @@
         <v>11</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I97" s="7" t="s">
         <v>12</v>
@@ -2630,10 +2623,10 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>20</v>
@@ -2648,7 +2641,7 @@
         <v>11</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I109" s="7" t="s">
         <v>12</v>
@@ -2863,10 +2856,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>20</v>
@@ -2881,7 +2874,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>12</v>
@@ -3071,10 +3064,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>20</v>
@@ -3089,7 +3082,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>12</v>
@@ -3279,10 +3272,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>20</v>
@@ -3297,7 +3290,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>12</v>
@@ -3487,10 +3480,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>20</v>
@@ -3505,7 +3498,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>12</v>
@@ -3695,10 +3688,10 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>20</v>
@@ -3713,7 +3706,7 @@
         <v>11</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>12</v>
@@ -3903,10 +3896,10 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>20</v>
@@ -3921,7 +3914,7 @@
         <v>11</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>12</v>
@@ -4111,10 +4104,10 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>20</v>
@@ -4129,7 +4122,7 @@
         <v>11</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>12</v>
@@ -4319,10 +4312,10 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>20</v>
@@ -4337,7 +4330,7 @@
         <v>11</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I85" s="7" t="s">
         <v>12</v>
@@ -4527,10 +4520,10 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>20</v>
@@ -4545,7 +4538,7 @@
         <v>11</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I97" s="7" t="s">
         <v>12</v>
@@ -4735,10 +4728,10 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>20</v>
@@ -4753,7 +4746,7 @@
         <v>11</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I109" s="7" t="s">
         <v>12</v>

</xml_diff>